<commit_message>
Added new things to the country file
</commit_message>
<xml_diff>
--- a/App Data - Country.xlsx
+++ b/App Data - Country.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Country Stats" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Country</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t>Totals</t>
+  </si>
+  <si>
+    <t>Mean Profits Made (US$)</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
   </si>
 </sst>
 </file>
@@ -503,19 +509,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D46"/>
+  <dimension ref="A2:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -525,8 +532,11 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -537,8 +547,19 @@
         <f>0.72*2</f>
         <v>1.44</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <f>D3/C3</f>
+        <v>0.72</v>
+      </c>
+      <c r="F3">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G3">
+        <f>(E3-F3)^2</f>
+        <v>8.2746466890572246E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -548,8 +569,19 @@
       <c r="D4">
         <v>43.68</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <f t="shared" ref="E3:F46" si="0">D4/C4</f>
+        <v>0.78</v>
+      </c>
+      <c r="F4">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G45" si="1">(E4-F4)^2</f>
+        <v>9.5883648905722171E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -559,8 +591,19 @@
       <c r="D5">
         <v>0.94</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.94</v>
+      </c>
+      <c r="F5">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>1.6650009289057219E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -570,8 +613,19 @@
       <c r="D6">
         <v>0.41299999999999998</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="F6">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>0.15837620887905723</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -581,8 +635,19 @@
       <c r="D7">
         <v>66.56</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>1.0084848484848485</v>
+      </c>
+      <c r="F7">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>3.9014056967110515E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -592,8 +657,19 @@
       <c r="D8">
         <v>1.82</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.91</v>
+      </c>
+      <c r="F8">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>9.807914389057237E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -603,8 +679,19 @@
       <c r="D9">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.95</v>
+      </c>
+      <c r="F9">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>1.9330707589057219E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -614,8 +701,19 @@
       <c r="D10">
         <v>5.73</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>1.1460000000000001</v>
+      </c>
+      <c r="F10">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>0.11224839426905733</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -625,8 +723,19 @@
       <c r="D11">
         <v>8.57</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0.9522222222222223</v>
+      </c>
+      <c r="F11">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>1.9953578816217749E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -636,8 +745,19 @@
       <c r="D12">
         <v>4.2699999999999996</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>1.0674999999999999</v>
+      </c>
+      <c r="F12">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>6.5810162614057185E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>13</v>
       </c>
@@ -647,8 +767,19 @@
       <c r="D13">
         <v>0.72</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0.72</v>
+      </c>
+      <c r="F13">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>8.2746466890572246E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>14</v>
       </c>
@@ -658,8 +789,19 @@
       <c r="D14">
         <v>0.72</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0.72</v>
+      </c>
+      <c r="F14">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>8.2746466890572246E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>15</v>
       </c>
@@ -669,8 +811,19 @@
       <c r="D15">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="F15">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>3.1553039200168338E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>16</v>
       </c>
@@ -680,8 +833,19 @@
       <c r="D16">
         <v>52.36</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0.88745762711864407</v>
+      </c>
+      <c r="F16">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>5.8511089997725406E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
@@ -691,8 +855,19 @@
       <c r="D17" s="2">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0.95</v>
+      </c>
+      <c r="F17">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>1.9330707589057219E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
@@ -702,8 +877,19 @@
       <c r="D18" s="2">
         <v>1.08</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>1.08</v>
+      </c>
+      <c r="F18">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>7.2379785489057283E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
@@ -713,8 +899,19 @@
       <c r="D19" s="2">
         <v>1.04</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>1.04</v>
+      </c>
+      <c r="F19">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>5.2456992289057251E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
@@ -724,8 +921,19 @@
       <c r="D20" s="2">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="F20">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>1.5237245890572253E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
@@ -735,16 +943,38 @@
       <c r="D21" s="3">
         <v>1.94</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>0.97</v>
+      </c>
+      <c r="F21">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>2.5292104189057224E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>0.65766436908905723</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
@@ -754,8 +984,19 @@
       <c r="D23" s="3">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>0.45</v>
+      </c>
+      <c r="F23">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>0.13029579258905719</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>24</v>
       </c>
@@ -765,8 +1006,19 @@
       <c r="D24" s="3">
         <v>1.88</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>0.94</v>
+      </c>
+      <c r="F24">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>1.6650009289057219E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>25</v>
       </c>
@@ -776,8 +1028,19 @@
       <c r="D25" s="3">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="F25">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>5.9681717200168329E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>26</v>
       </c>
@@ -787,8 +1050,19 @@
       <c r="D26" s="3">
         <v>3.08</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>0.77</v>
+      </c>
+      <c r="F26">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>1.6781381890572215E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>27</v>
       </c>
@@ -798,24 +1072,57 @@
       <c r="D27" s="3">
         <v>5.86</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>0.97666666666666668</v>
+      </c>
+      <c r="F27">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>2.7457014166835016E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>0.65766436908905723</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>0.65766436908905723</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>30</v>
       </c>
@@ -825,8 +1132,19 @@
       <c r="D30" s="3">
         <v>0.92</v>
       </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>0.92</v>
+      </c>
+      <c r="F30">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>1.188861268905724E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>31</v>
       </c>
@@ -836,8 +1154,19 @@
       <c r="D31" s="3">
         <v>3.43</v>
       </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>0.85750000000000004</v>
+      </c>
+      <c r="F31">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>2.1654983140572313E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>32</v>
       </c>
@@ -847,8 +1176,19 @@
       <c r="D32" s="3">
         <v>2.15</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>1.075</v>
+      </c>
+      <c r="F32">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>6.9714436339057217E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>33</v>
       </c>
@@ -858,16 +1198,38 @@
       <c r="D33" s="3">
         <v>1.96</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>0.98</v>
+      </c>
+      <c r="F33">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>2.8572802489057227E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>0.65766436908905723</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>35</v>
       </c>
@@ -877,8 +1239,19 @@
       <c r="D35" s="3">
         <v>0.82</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>0.82</v>
+      </c>
+      <c r="F35">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>8.1629689057224582E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>36</v>
       </c>
@@ -888,8 +1261,19 @@
       <c r="D36" s="3">
         <v>1.96</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>0.49</v>
+      </c>
+      <c r="F36">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>0.10301858578905722</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>37</v>
       </c>
@@ -899,8 +1283,19 @@
       <c r="D37" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>0.65766436908905723</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
         <v>38</v>
       </c>
@@ -910,8 +1305,19 @@
       <c r="D38" s="3">
         <v>0.94</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>0.94</v>
+      </c>
+      <c r="F38">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>1.6650009289057219E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>39</v>
       </c>
@@ -921,8 +1327,19 @@
       <c r="D39" s="3">
         <v>6.6</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="F39">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>1.9697883905722447E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
         <v>40</v>
       </c>
@@ -932,8 +1349,19 @@
       <c r="D40" s="3">
         <v>1.1200000000000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="F40">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="1"/>
+        <v>9.5502578689057302E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
         <v>41</v>
       </c>
@@ -943,8 +1371,19 @@
       <c r="D41" s="3">
         <v>1.04</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>1.04</v>
+      </c>
+      <c r="F41">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="1"/>
+        <v>5.2456992289057251E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
         <v>42</v>
       </c>
@@ -954,8 +1393,19 @@
       <c r="D42" s="3">
         <v>2.2799999999999998</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="F42">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="1"/>
+        <v>0.10826397528905718</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
         <v>43</v>
       </c>
@@ -965,16 +1415,38 @@
       <c r="D43" s="3">
         <v>1899.04</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>0.806044142614601</v>
+      </c>
+      <c r="F43">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="1"/>
+        <v>2.4215673960416146E-5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C44">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="1"/>
+        <v>0.65766436908905723</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
         <v>45</v>
       </c>
@@ -984,8 +1456,19 @@
       <c r="D45" s="3">
         <v>4.33</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>0.54125000000000001</v>
+      </c>
+      <c r="F45">
+        <v>0.81096508499999997</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="1"/>
+        <v>7.2746227076557202E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -1001,8 +1484,25 @@
         <f>SUM(D3:D45)</f>
         <v>2136.893</v>
       </c>
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>0.81096508538899437</v>
+      </c>
+      <c r="F46">
+        <v>0.81096508499999997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48">
+        <f>SQRT(SUM(G3:G45)/43)</f>
+        <v>0.35497765079134769</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added some things to the country file
</commit_message>
<xml_diff>
--- a/App Data - Country.xlsx
+++ b/App Data - Country.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Country</t>
   </si>
@@ -171,6 +171,24 @@
   </si>
   <si>
     <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>Difference between mean</t>
+  </si>
+  <si>
+    <t>95% Confidence(+/-)</t>
+  </si>
+  <si>
+    <t>Upper Limit</t>
+  </si>
+  <si>
+    <t>Lower Limit</t>
+  </si>
+  <si>
+    <t>Standardized for Currency:</t>
   </si>
 </sst>
 </file>
@@ -233,7 +251,54 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -244,6 +309,25 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:G45" totalsRowShown="0">
+  <autoFilter ref="B2:G45"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Country" dataDxfId="1"/>
+    <tableColumn id="2" name="Transactions Made"/>
+    <tableColumn id="3" name="Profits Made (US$)" dataDxfId="0"/>
+    <tableColumn id="4" name="Mean Profits Made (US$)">
+      <calculatedColumnFormula>D3/C3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="mean"/>
+    <tableColumn id="6" name="Difference between mean">
+      <calculatedColumnFormula>(E3-F3)^2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -509,17 +593,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G48"/>
+  <dimension ref="A2:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
@@ -535,6 +622,12 @@
       <c r="E2" t="s">
         <v>47</v>
       </c>
+      <c r="F2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -570,7 +663,7 @@
         <v>43.68</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E3:F46" si="0">D4/C4</f>
+        <f t="shared" ref="E4:E46" si="0">D4/C4</f>
         <v>0.78</v>
       </c>
       <c r="F4">
@@ -1501,8 +1594,49 @@
         <v>0.35497765079134769</v>
       </c>
     </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49">
+        <f>_xlfn.CONFIDENCE.NORM(0.05, D48,43)</f>
+        <v>0.10609987547565078</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>53</v>
+      </c>
+      <c r="D50">
+        <f>F46-D49</f>
+        <v>0.70486520952434917</v>
+      </c>
+      <c r="E50" t="s">
+        <v>52</v>
+      </c>
+      <c r="F50">
+        <f>F45+D49</f>
+        <v>0.91706496047565078</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>54</v>
+      </c>
+      <c r="D51">
+        <f>0.7</f>
+        <v>0.7</v>
+      </c>
+      <c r="E51">
+        <f>0.91</f>
+        <v>0.91</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>